<commit_message>
theme change for gantt chart + more report content added
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="project" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="project" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Actual">(PeriodInActual*(project!$E1&gt;0))*PeriodInPlan</definedName>
@@ -667,11 +668,801 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="316979120"/>
+        <c:axId val="316974856"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="316979120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="316974856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="316974856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="316979120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -683,8 +1474,8 @@
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>14</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:col>15</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>257175</xdr:rowOff>
         </xdr:to>
@@ -726,7 +1517,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Violet II">
+    <a:clrScheme name="Aspect">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -734,34 +1525,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="632E62"/>
+        <a:srgbClr val="323232"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EAE5EB"/>
+        <a:srgbClr val="E3DED1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="92278F"/>
+        <a:srgbClr val="F07F09"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="9B57D3"/>
+        <a:srgbClr val="9F2936"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="755DD9"/>
+        <a:srgbClr val="1B587C"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="665EB8"/>
+        <a:srgbClr val="4E8542"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="45A5ED"/>
+        <a:srgbClr val="604878"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="5982DB"/>
+        <a:srgbClr val="C19859"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0066FF"/>
+        <a:srgbClr val="6B9F25"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="666699"/>
+        <a:srgbClr val="B26B02"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Project Planner Gantt">
@@ -955,8 +1746,8 @@
   </sheetPr>
   <dimension ref="B2:BQ34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BW13" sqref="BW13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BZ19" sqref="BZ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>

</xml_diff>